<commit_message>
Further analysis and refinement of study data
</commit_message>
<xml_diff>
--- a/docs/evaluation/user-study/analysis/evaluation-data-synthesized.xlsx
+++ b/docs/evaluation/user-study/analysis/evaluation-data-synthesized.xlsx
@@ -5,20 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\adr-manager\docs\evaluation\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\adr-manager\docs\evaluation\user-study\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD9DF20-9B5B-4043-88B2-EC874EA2AC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019BFA95-D66A-4ED9-A8A7-BEFD317B6913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0661121A-785B-47D4-B27B-0D2BD6FC24AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0661121A-785B-47D4-B27B-0D2BD6FC24AE}"/>
   </bookViews>
   <sheets>
     <sheet name="CleanData" sheetId="1" r:id="rId1"/>
     <sheet name="functionality" sheetId="2" r:id="rId2"/>
+    <sheet name="usability" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CleanData!$A$1:$G$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">functionality!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">usability!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="169">
   <si>
     <t>Efficiency of User Interface</t>
   </si>
@@ -974,21 +976,12 @@
     <t>existing feature</t>
   </si>
   <si>
-    <t>If the parser in the convert tab has problems, changed content is lost.</t>
-  </si>
-  <si>
-    <t>Usage as an IDE plugin</t>
-  </si>
-  <si>
     <t>Timeline/history of a decision (e.g. first Selenium was used, later switched to Cypress)</t>
   </si>
   <si>
     <t>Linking decisions to other decisions</t>
   </si>
   <si>
-    <t>Supporting images</t>
-  </si>
-  <si>
     <t>3, 4, 6, 7, 8</t>
   </si>
   <si>
@@ -1016,12 +1009,6 @@
     <t>Spelling correction</t>
   </si>
   <si>
-    <t>Supporting GitLab</t>
-  </si>
-  <si>
-    <t>Supporting superseding / deprecation of ADRs and navigating between these ADRs</t>
-  </si>
-  <si>
     <t>Adding new deciders dynamically like options</t>
   </si>
   <si>
@@ -1092,6 +1079,177 @@
   </si>
   <si>
     <t>Import &amp; export</t>
+  </si>
+  <si>
+    <t>Supporting images in an ADR</t>
+  </si>
+  <si>
+    <t>Supporting different Git platforms (GitLab, Azure DevOps, Bitbucket)</t>
+  </si>
+  <si>
+    <t>3, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>Switching between navigate editor fields with the tabulator key</t>
+  </si>
+  <si>
+    <t>Superseding / deprecating ADRs and navigating between them</t>
+  </si>
+  <si>
+    <t>Prevent content loss if the parser in the convert tab has problems</t>
+  </si>
+  <si>
+    <t>Usage as an IDE plugin (VS Code)</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>understandability</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>4, 7</t>
+  </si>
+  <si>
+    <t>6, 9</t>
+  </si>
+  <si>
+    <t>2, 9</t>
+  </si>
+  <si>
+    <t>3, 7</t>
+  </si>
+  <si>
+    <t>2, 7</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>2, 3, 8</t>
+  </si>
+  <si>
+    <t>3, 4, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 6, 7, 8</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 6, 9</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>1, 8, 9</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 5, 6, 9</t>
+  </si>
+  <si>
+    <t>Advanced mode is not required</t>
+  </si>
+  <si>
+    <t>Preview of the formatted markdown is good</t>
+  </si>
+  <si>
+    <t>Push dialog was understandable</t>
+  </si>
+  <si>
+    <t>Pure Markdown may be faster than the MADR editor</t>
+  </si>
+  <si>
+    <t>Efficient usage (the UI is fast and clearly structured)</t>
+  </si>
+  <si>
+    <t>Editor modes are not clear (scopes and differences)</t>
+  </si>
+  <si>
+    <t>Data persistence unclear (auto-save?)</t>
+  </si>
+  <si>
+    <t>Uncertainty if Markdown should be used in editor fields</t>
+  </si>
+  <si>
+    <t>Automatic extension of lists was not clear (copy &amp; paste problem)</t>
+  </si>
+  <si>
+    <t>Copy &amp; paste is not well supported (especially in lists)</t>
+  </si>
+  <si>
+    <t>When knowing the workflow and modes, the efficiency is okay</t>
+  </si>
+  <si>
+    <t>More efficient than having to write Markdown</t>
+  </si>
+  <si>
+    <t>Web application is prettier for meetings than raw Markdown</t>
+  </si>
+  <si>
+    <t>An IDE plugin would be more efficient (VS Code)</t>
+  </si>
+  <si>
+    <t>Expand feature of "considered options" is hard to see</t>
+  </si>
+  <si>
+    <t>Too few labels and tool tips (unclear UI elements)</t>
+  </si>
+  <si>
+    <t>Navigation from the "Convert tab" is unclear (how to cancel?)</t>
+  </si>
+  <si>
+    <t>"Commit and push" button is hard to find</t>
+  </si>
+  <si>
+    <t>Default text of the "because" field in "decision outcome" is confusing</t>
+  </si>
+  <si>
+    <t>Missing an intro text explaining what ADRs are for</t>
+  </si>
+  <si>
+    <t>Uncertainty how adding a repository works (is it a local one?)</t>
+  </si>
+  <si>
+    <t>"Commit and push" button too close to "remove repository" button</t>
+  </si>
+  <si>
+    <t>"Commit and push" icon may be confusing</t>
+  </si>
+  <si>
+    <t>Deletion of "options" should give a warning</t>
+  </si>
+  <si>
+    <t>No indication that some elements are lists</t>
+  </si>
+  <si>
+    <t>Some multi-line text fields are too small</t>
+  </si>
+  <si>
+    <t>"Deciders" need a description and should behave like a list</t>
+  </si>
+  <si>
+    <t>Modes don't support workflow and are hard to understand</t>
+  </si>
+  <si>
+    <t>"New ADR" button is so big that ADR could also be written out</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Application is generally intuitive and well understandable</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1720,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C185EBEA-B074-46D9-9F31-F4869C518936}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,10 +2107,10 @@
         <v>64</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>65</v>
@@ -1966,7 +2124,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>76</v>
@@ -1987,13 +2145,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D3">
         <f>LEN(E3)-LEN(SUBSTITUTE(E3,",", "")) + 1</f>
@@ -2008,13 +2166,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D4">
         <f>LEN(E4)-LEN(SUBSTITUTE(E4,",", "")) + 1</f>
@@ -2029,20 +2187,20 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <f>LEN(E5)-LEN(SUBSTITUTE(E5,",", "")) + 1</f>
         <v>5</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -2050,20 +2208,20 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <f>LEN(E6)-LEN(SUBSTITUTE(E6,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
         <v>72</v>
@@ -2071,13 +2229,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <f>LEN(E7)-LEN(SUBSTITUTE(E7,",", "")) + 1</f>
@@ -2092,13 +2250,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <f>LEN(E8)-LEN(SUBSTITUTE(E8,",", "")) + 1</f>
@@ -2113,13 +2271,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <f>LEN(E9)-LEN(SUBSTITUTE(E9,",", "")) + 1</f>
@@ -2134,62 +2292,62 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D10">
         <f>LEN(E10)-LEN(SUBSTITUTE(E10,",", "")) + 1</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D11">
         <f>LEN(E11)-LEN(SUBSTITUTE(E11,",", "")) + 1</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="10">
         <v>2</v>
       </c>
+      <c r="E11" s="10" t="s">
+        <v>119</v>
+      </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
         <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D12">
         <f>LEN(E12)-LEN(SUBSTITUTE(E12,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E12" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>73</v>
@@ -2203,7 +2361,7 @@
         <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <f>LEN(E13)-LEN(SUBSTITUTE(E13,",", "")) + 1</f>
@@ -2218,13 +2376,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <f>LEN(E14)-LEN(SUBSTITUTE(E14,",", "")) + 1</f>
@@ -2239,13 +2397,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D15">
         <f>LEN(E15)-LEN(SUBSTITUTE(E15,",", "")) + 1</f>
@@ -2260,13 +2418,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D16">
         <f>LEN(E16)-LEN(SUBSTITUTE(E16,",", "")) + 1</f>
@@ -2281,13 +2439,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D17">
         <f>LEN(E17)-LEN(SUBSTITUTE(E17,",", "")) + 1</f>
@@ -2302,13 +2460,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
         <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D18">
         <f>LEN(E18)-LEN(SUBSTITUTE(E18,",", "")) + 1</f>
@@ -2323,13 +2481,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
         <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D19">
         <f>LEN(E19)-LEN(SUBSTITUTE(E19,",", "")) + 1</f>
@@ -2344,13 +2502,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D20">
         <f>LEN(E20)-LEN(SUBSTITUTE(E20,",", "")) + 1</f>
@@ -2365,13 +2523,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <f>LEN(E21)-LEN(SUBSTITUTE(E21,",", "")) + 1</f>
@@ -2386,13 +2544,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
         <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D22">
         <f>LEN(E22)-LEN(SUBSTITUTE(E22,",", "")) + 1</f>
@@ -2407,20 +2565,20 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
         <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D23">
         <f>LEN(E23)-LEN(SUBSTITUTE(E23,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E23" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
         <v>72</v>
@@ -2428,62 +2586,62 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D24">
         <f>LEN(E24)-LEN(SUBSTITUTE(E24,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E24" s="10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D25">
         <f>LEN(E25)-LEN(SUBSTITUTE(E25,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E25" s="10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
         <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D26">
         <f>LEN(E26)-LEN(SUBSTITUTE(E26,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E26" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
         <v>73</v>
@@ -2491,41 +2649,41 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
         <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D27">
         <f>LEN(E27)-LEN(SUBSTITUTE(E27,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E27" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D28">
         <f>LEN(E28)-LEN(SUBSTITUTE(E28,",", "")) + 1</f>
-        <v>2</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>97</v>
+        <v>1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>6</v>
       </c>
       <c r="F28" t="s">
         <v>72</v>
@@ -2533,27 +2691,45 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D29">
         <f>LEN(E29)-LEN(SUBSTITUTE(E29,",", "")) + 1</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="F29" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="10"/>
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30">
+        <f>LEN(E30)-LEN(SUBSTITUTE(E30,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
@@ -2569,6 +2745,9 @@
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{C185EBEA-B074-46D9-9F31-F4869C518936}">
@@ -2579,4 +2758,603 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A133090-482F-485B-84D7-BC94F7B4B37F}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2">
+        <f>LEN(F2)-LEN(SUBSTITUTE(F2,",", "")) + 1</f>
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3">
+        <f>LEN(F3)-LEN(SUBSTITUTE(F3,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4">
+        <f>LEN(F4)-LEN(SUBSTITUTE(F4,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5">
+        <f>LEN(F5)-LEN(SUBSTITUTE(F5,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <f>LEN(F6)-LEN(SUBSTITUTE(F6,",", "")) + 1</f>
+        <v>6</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7">
+        <f>LEN(F7)-LEN(SUBSTITUTE(F7,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8">
+        <f>LEN(F8)-LEN(SUBSTITUTE(F8,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9">
+        <f>LEN(F9)-LEN(SUBSTITUTE(F9,",", "")) + 1</f>
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10">
+        <f>LEN(F10)-LEN(SUBSTITUTE(F10,",", "")) + 1</f>
+        <v>6</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11">
+        <f>LEN(F11)-LEN(SUBSTITUTE(F11,",", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12">
+        <f>LEN(F12)-LEN(SUBSTITUTE(F12,",", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13">
+        <f>LEN(F13)-LEN(SUBSTITUTE(F13,",", "")) + 1</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14">
+        <f>LEN(F14)-LEN(SUBSTITUTE(F14,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15">
+        <f>LEN(F15)-LEN(SUBSTITUTE(F15,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16">
+        <f>LEN(F16)-LEN(SUBSTITUTE(F16,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17">
+        <f>LEN(F17)-LEN(SUBSTITUTE(F17,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18">
+        <f>LEN(F18)-LEN(SUBSTITUTE(F18,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19">
+        <f>LEN(F19)-LEN(SUBSTITUTE(F19,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20">
+        <f>LEN(F20)-LEN(SUBSTITUTE(F20,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21">
+        <f>LEN(F21)-LEN(SUBSTITUTE(F21,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22">
+        <f>LEN(F22)-LEN(SUBSTITUTE(F22,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23">
+        <f>LEN(F23)-LEN(SUBSTITUTE(F23,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24">
+        <f>LEN(F24)-LEN(SUBSTITUTE(F24,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25">
+        <f>LEN(F25)-LEN(SUBSTITUTE(F25,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26">
+        <f>LEN(F26)-LEN(SUBSTITUTE(F26,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27">
+        <f>LEN(F27)-LEN(SUBSTITUTE(F27,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28">
+        <f>LEN(F28)-LEN(SUBSTITUTE(F28,",", "")) + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29">
+        <f>LEN(F29)-LEN(SUBSTITUTE(F29,",", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30">
+        <f>LEN(F30)-LEN(SUBSTITUTE(F30,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31">
+        <f>LEN(F31)-LEN(SUBSTITUTE(F31,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="10">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{6A133090-482F-485B-84D7-BC94F7B4B37F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F34">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added analysis script, refined evaluation synthesis
</commit_message>
<xml_diff>
--- a/docs/evaluation/user-study/analysis/evaluation-data-synthesized.xlsx
+++ b/docs/evaluation/user-study/analysis/evaluation-data-synthesized.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\adr-manager\docs\evaluation\user-study\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\adr-manager\docs\evaluation\user-study\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF2D0D8-D713-4E81-B2BE-A0F22A13ACB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679332E7-5BCC-4CC1-9686-E83601DA2D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0661121A-785B-47D4-B27B-0D2BD6FC24AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0661121A-785B-47D4-B27B-0D2BD6FC24AE}"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>Expand feature of "considered options" is hard to see</t>
   </si>
   <si>
-    <t>Too few labels and tool tips (unclear UI elements)</t>
-  </si>
-  <si>
     <t>Navigation from the "Convert tab" is unclear (how to cancel?)</t>
   </si>
   <si>
@@ -294,15 +291,9 @@
     <t>Some multi-line text fields are too small</t>
   </si>
   <si>
-    <t>"Deciders" need a description and should behave like a list</t>
-  </si>
-  <si>
     <t>"New ADR" button is so big that ADR could also be written out</t>
   </si>
   <si>
-    <t>Application is generally intuitive and well understandable</t>
-  </si>
-  <si>
     <t>IDE plugin</t>
   </si>
   <si>
@@ -532,6 +523,15 @@
   </si>
   <si>
     <t>Task Duration (min)</t>
+  </si>
+  <si>
+    <t>"Deciders" needs a description and should behave like a list</t>
+  </si>
+  <si>
+    <t>Application is generally intuitive and easy to understand</t>
+  </si>
+  <si>
+    <t>Too few labels and tooltips (unclear UI elements)</t>
   </si>
 </sst>
 </file>
@@ -915,80 +915,80 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
         <v>117</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>120</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -997,16 +997,16 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J2">
         <v>18</v>
@@ -1021,18 +1021,18 @@
         <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D3">
         <v>32</v>
@@ -1041,16 +1041,16 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" t="s">
         <v>122</v>
       </c>
-      <c r="G3" t="s">
-        <v>125</v>
-      </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J3">
         <v>18</v>
@@ -1065,18 +1065,18 @@
         <v>5</v>
       </c>
       <c r="N3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1085,16 +1085,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J4">
         <v>13</v>
@@ -1109,18 +1109,18 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1129,16 +1129,16 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" t="s">
         <v>138</v>
       </c>
-      <c r="H5" t="s">
-        <v>141</v>
-      </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J5">
         <v>14</v>
@@ -1153,18 +1153,18 @@
         <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1173,16 +1173,16 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J6">
         <v>18</v>
@@ -1197,18 +1197,18 @@
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -1217,16 +1217,16 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J7">
         <v>11</v>
@@ -1241,18 +1241,18 @@
         <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -1261,16 +1261,16 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J8">
         <v>10</v>
@@ -1285,18 +1285,18 @@
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D9">
         <v>20</v>
@@ -1305,16 +1305,16 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J9">
         <v>20</v>
@@ -1329,18 +1329,18 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1349,16 +1349,16 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" t="s">
         <v>140</v>
       </c>
-      <c r="H10" t="s">
-        <v>143</v>
-      </c>
       <c r="I10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J10">
         <v>9</v>
@@ -1373,10 +1373,10 @@
         <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="J13" s="4"/>
@@ -1384,9 +1384,9 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D14">
         <f>MEDIAN(D2:D10)</f>
@@ -1397,7 +1397,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J14">
         <f>MEDIAN(J2:J10)</f>
@@ -1422,9 +1422,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D15" s="5">
         <f>AVERAGE(D2:D10)</f>
@@ -1435,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J15" s="5">
         <f>AVERAGE(J2:J10)</f>
@@ -1465,22 +1465,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C185EBEA-B074-46D9-9F31-F4869C518936}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="112.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="112.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1497,37 +1495,37 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D30" si="0">LEN(E2)-LEN(SUBSTITUTE(E2,",", "")) + 1</f>
+        <f>LEN(E2)-LEN(SUBSTITUTE(E2,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1535,10 +1533,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>LEN(E3)-LEN(SUBSTITUTE(E3,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E3" s="1">
@@ -1548,21 +1546,21 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>LEN(E4)-LEN(SUBSTITUTE(E4,",", "")) + 1</f>
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1575,7 +1573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1586,7 +1584,7 @@
         <v>38</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>LEN(E5)-LEN(SUBSTITUTE(E5,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E5" s="1">
@@ -1596,10 +1594,10 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>38</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>LEN(E6)-LEN(SUBSTITUTE(E6,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E6" s="1">
@@ -1620,10 +1618,10 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1634,7 +1632,7 @@
         <v>37</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>LEN(E7)-LEN(SUBSTITUTE(E7,",", "")) + 1</f>
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1644,10 +1642,10 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1658,20 +1656,20 @@
         <v>37</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>LEN(E8)-LEN(SUBSTITUTE(E8,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1682,20 +1680,20 @@
         <v>37</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>LEN(E9)-LEN(SUBSTITUTE(E9,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1706,20 +1704,20 @@
         <v>37</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>LEN(E10)-LEN(SUBSTITUTE(E10,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E10" s="1">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1730,20 +1728,20 @@
         <v>37</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>LEN(E11)-LEN(SUBSTITUTE(E11,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1751,23 +1749,23 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f>LEN(E12)-LEN(SUBSTITUTE(E12,",", "")) + 1</f>
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1775,23 +1773,23 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>LEN(E13)-LEN(SUBSTITUTE(E13,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1799,10 +1797,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>LEN(E14)-LEN(SUBSTITUTE(E14,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E14" s="1">
@@ -1812,250 +1810,250 @@
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>LEN(E15)-LEN(SUBSTITUTE(E15,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>LEN(E16)-LEN(SUBSTITUTE(E16,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f>LEN(E17)-LEN(SUBSTITUTE(E17,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="G17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>LEN(E18)-LEN(SUBSTITUTE(E18,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="G18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>LEN(E19)-LEN(SUBSTITUTE(E19,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f>LEN(E20)-LEN(SUBSTITUTE(E20,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>LEN(E21)-LEN(SUBSTITUTE(E21,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>LEN(E22)-LEN(SUBSTITUTE(E22,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>LEN(E23)-LEN(SUBSTITUTE(E23,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>LEN(E24)-LEN(SUBSTITUTE(E24,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2063,23 +2061,23 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>LEN(E25)-LEN(SUBSTITUTE(E25,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E25" s="1">
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2087,10 +2085,10 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f>LEN(E26)-LEN(SUBSTITUTE(E26,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E26" s="1">
@@ -2100,10 +2098,10 @@
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2111,10 +2109,10 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f>LEN(E27)-LEN(SUBSTITUTE(E27,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E27" s="1">
@@ -2124,10 +2122,10 @@
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2135,10 +2133,10 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>LEN(E28)-LEN(SUBSTITUTE(E28,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E28" s="1">
@@ -2148,10 +2146,10 @@
         <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2159,10 +2157,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>LEN(E29)-LEN(SUBSTITUTE(E29,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -2172,10 +2170,10 @@
         <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2183,42 +2181,46 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>LEN(E30)-LEN(SUBSTITUTE(E30,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G30" xr:uid="{C185EBEA-B074-46D9-9F31-F4869C518936}"/>
+  <autoFilter ref="A1:G30" xr:uid="{C185EBEA-B074-46D9-9F31-F4869C518936}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G30">
+      <sortCondition ref="B1:B30"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
     <sortCondition ref="B2:B30"/>
     <sortCondition ref="C2:C30"/>
@@ -2233,22 +2235,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A133090-482F-485B-84D7-BC94F7B4B37F}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2268,10 +2268,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2279,23 +2279,23 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E31" si="0">LEN(F2)-LEN(SUBSTITUTE(F2,",", "")) + 1</f>
+        <f>LEN(F2)-LEN(SUBSTITUTE(F2,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -2303,13 +2303,13 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>LEN(F3)-LEN(SUBSTITUTE(F3,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -2319,21 +2319,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>LEN(F4)-LEN(SUBSTITUTE(F4,",", "")) + 1</f>
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -2343,7 +2343,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -2351,13 +2351,13 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
         <v>50</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>LEN(F5)-LEN(SUBSTITUTE(F5,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F5" s="1">
@@ -2367,21 +2367,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>LEN(F6)-LEN(SUBSTITUTE(F6,",", "")) + 1</f>
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -2391,21 +2391,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>LEN(F7)-LEN(SUBSTITUTE(F7,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -2415,21 +2415,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>48</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>LEN(F8)-LEN(SUBSTITUTE(F8,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F8" s="1">
@@ -2439,7 +2439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -2447,23 +2447,23 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>LEN(F9)-LEN(SUBSTITUTE(F9,",", "")) + 1</f>
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2471,239 +2471,239 @@
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>LEN(F10)-LEN(SUBSTITUTE(F10,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>LEN(F11)-LEN(SUBSTITUTE(F11,",", "")) + 1</f>
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>LEN(F12)-LEN(SUBSTITUTE(F12,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F12" s="1">
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
         <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>LEN(F13)-LEN(SUBSTITUTE(F13,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F13" s="1">
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>LEN(F14)-LEN(SUBSTITUTE(F14,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>LEN(F15)-LEN(SUBSTITUTE(F15,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F15" s="1">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
         <v>48</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>LEN(F16)-LEN(SUBSTITUTE(F16,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F16" s="1">
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
         <v>48</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3</v>
+        <f>LEN(F17)-LEN(SUBSTITUTE(F17,",", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
         <v>48</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f>LEN(F18)-LEN(SUBSTITUTE(F18,",", "")) + 1</f>
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
         <v>48</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>LEN(F19)-LEN(SUBSTITUTE(F19,",", "")) + 1</f>
+        <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -2711,47 +2711,47 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
+        <f>LEN(F20)-LEN(SUBSTITUTE(F20,",", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>LEN(F21)-LEN(SUBSTITUTE(F21,",", "")) + 1</f>
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2759,47 +2759,47 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>LEN(F22)-LEN(SUBSTITUTE(F22,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>LEN(F23)-LEN(SUBSTITUTE(F23,",", "")) + 1</f>
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2807,47 +2807,47 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
         <v>48</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>LEN(F24)-LEN(SUBSTITUTE(F24,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f>LEN(F25)-LEN(SUBSTITUTE(F25,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F25" s="1">
         <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2855,13 +2855,13 @@
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
         <v>50</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f>LEN(F26)-LEN(SUBSTITUTE(F26,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F26" s="1">
@@ -2871,7 +2871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2879,23 +2879,23 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>48</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f>LEN(F27)-LEN(SUBSTITUTE(F27,",", "")) + 1</f>
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2903,13 +2903,13 @@
         <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
         <v>50</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f>LEN(F28)-LEN(SUBSTITUTE(F28,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F28" s="1">
@@ -2919,7 +2919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2927,13 +2927,13 @@
         <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D29" t="s">
         <v>50</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f>LEN(F29)-LEN(SUBSTITUTE(F29,",", "")) + 1</f>
         <v>1</v>
       </c>
       <c r="F29" s="1">
@@ -2943,60 +2943,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>50</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f>LEN(F30)-LEN(SUBSTITUTE(F30,",", "")) + 1</f>
         <v>5</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
         <v>48</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f>LEN(F31)-LEN(SUBSTITUTE(F31,",", "")) + 1</f>
         <v>4</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G31" xr:uid="{6A133090-482F-485B-84D7-BC94F7B4B37F}"/>
+  <autoFilter ref="A1:G31" xr:uid="{6A133090-482F-485B-84D7-BC94F7B4B37F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
+      <sortCondition ref="B1:B31"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F4 F11" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>